<commit_message>
reviewOrder change from dropdownlist to checkbox
- changed review orders scheduling function from dropdownbox to checkbox.
added a button for user to
- schedule/unschedule all orders function
</commit_message>
<xml_diff>
--- a/Content/manufacturingExcelImport.xlsx
+++ b/Content/manufacturingExcelImport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\source\repos\VentureScheduler\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADFE0E9-2337-4903-8109-7F2C2944DD80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DBDDC1-DEDE-4E34-BFEE-48A4B9BEEABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6458" yWindow="1290" windowWidth="9375" windowHeight="9465" xr2:uid="{C73AA913-6937-4929-98AB-0F68CDF14B3D}"/>
+    <workbookView xWindow="712" yWindow="1373" windowWidth="19261" windowHeight="9855" xr2:uid="{C73AA913-6937-4929-98AB-0F68CDF14B3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
   <si>
     <t>no</t>
   </si>
@@ -81,18 +81,9 @@
     <t>G5_46X7155_B_L8</t>
   </si>
   <si>
-    <t>SMT_Line_1                    </t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
-    <t>SMT_Line_2                    </t>
-  </si>
-  <si>
-    <t>SMT_Line_3                    </t>
-  </si>
-  <si>
     <t>Invalid cycle time</t>
   </si>
   <si>
@@ -124,6 +115,45 @@
   </si>
   <si>
     <t>New entry  (Product does not exist)</t>
+  </si>
+  <si>
+    <t>G6_00V6897_T_L8</t>
+  </si>
+  <si>
+    <t>G6_00V6900_B_L8</t>
+  </si>
+  <si>
+    <t>G6_00V6907_T_L8</t>
+  </si>
+  <si>
+    <t>G6_00V6910_T_L8</t>
+  </si>
+  <si>
+    <t>G7_00MJ518_B_L8</t>
+  </si>
+  <si>
+    <t>G7_00MJ521_B_L8</t>
+  </si>
+  <si>
+    <t>G8_00VJ679_B_L8</t>
+  </si>
+  <si>
+    <t>SMT_Line_8                    </t>
+  </si>
+  <si>
+    <t>SMT_Line_9                    </t>
+  </si>
+  <si>
+    <t>SMT_Line_10                    </t>
+  </si>
+  <si>
+    <t>SMT_Line_11                    </t>
+  </si>
+  <si>
+    <t>SMT_Line_12                    </t>
+  </si>
+  <si>
+    <t>SMT_Line_12                   </t>
   </si>
 </sst>
 </file>
@@ -476,19 +506,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74538F07-B388-4B5D-9587-60CA9861A8F4}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="20.796875" customWidth="1"/>
     <col min="3" max="3" width="15.86328125" customWidth="1"/>
-    <col min="4" max="4" width="20.53125" customWidth="1"/>
-    <col min="6" max="6" width="24.265625" customWidth="1"/>
-    <col min="7" max="7" width="19.46484375" customWidth="1"/>
+    <col min="4" max="4" width="6.1328125" customWidth="1"/>
+    <col min="6" max="6" width="14.53125" customWidth="1"/>
+    <col min="7" max="7" width="8.53125" customWidth="1"/>
     <col min="10" max="10" width="36" customWidth="1"/>
   </cols>
   <sheetData>
@@ -521,7 +551,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -541,7 +571,7 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="G2">
         <v>54</v>
@@ -553,7 +583,7 @@
         <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
@@ -573,7 +603,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G3">
         <v>65</v>
@@ -585,62 +615,62 @@
         <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
+      </c>
+      <c r="H4" s="1">
+        <v>43822</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
         <v>19</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>43822</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="G5">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="H5" s="1">
         <v>43822</v>
@@ -649,30 +679,30 @@
         <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="G6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
         <v>43822</v>
@@ -681,30 +711,30 @@
         <v>12</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G7">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="H7" s="1">
         <v>43822</v>
@@ -713,7 +743,7 @@
         <v>12</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
@@ -721,10 +751,10 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -733,7 +763,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G8">
         <v>543</v>
@@ -745,7 +775,210 @@
         <v>12</v>
       </c>
       <c r="J8" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9">
+        <v>76</v>
+      </c>
+      <c r="H9" s="1">
+        <v>43822</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10">
+        <v>76</v>
+      </c>
+      <c r="H10" s="1">
+        <v>43822</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11">
+        <v>53</v>
+      </c>
+      <c r="H11" s="1">
+        <v>43822</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12">
+        <v>82</v>
+      </c>
+      <c r="H12" s="1">
+        <v>43822</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13">
+        <v>63</v>
+      </c>
+      <c r="H13" s="1">
+        <v>43822</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14">
+        <v>63</v>
+      </c>
+      <c r="H14" s="1">
+        <v>43822</v>
+      </c>
+      <c r="I14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15">
+        <v>63</v>
+      </c>
+      <c r="H15" s="1">
+        <v>43822</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update all back to list pages
</commit_message>
<xml_diff>
--- a/Content/manufacturingExcelImport.xlsx
+++ b/Content/manufacturingExcelImport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\source\repos\VentureScheduler\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DBDDC1-DEDE-4E34-BFEE-48A4B9BEEABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5098C1-99EA-4E93-B9F7-541DC64BDD78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="712" yWindow="1373" windowWidth="19261" windowHeight="9855" xr2:uid="{C73AA913-6937-4929-98AB-0F68CDF14B3D}"/>
+    <workbookView xWindow="712" yWindow="772" windowWidth="18330" windowHeight="10441" xr2:uid="{C73AA913-6937-4929-98AB-0F68CDF14B3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Final commit and update
</commit_message>
<xml_diff>
--- a/Content/manufacturingExcelImport.xlsx
+++ b/Content/manufacturingExcelImport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\source\repos\VentureScheduler\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5098C1-99EA-4E93-B9F7-541DC64BDD78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58C52BA-9812-48E4-8E5E-5FAF1C8F665D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="712" yWindow="772" windowWidth="18330" windowHeight="10441" xr2:uid="{C73AA913-6937-4929-98AB-0F68CDF14B3D}"/>
+    <workbookView xWindow="0" yWindow="1688" windowWidth="13680" windowHeight="10440" xr2:uid="{C73AA913-6937-4929-98AB-0F68CDF14B3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
   <si>
     <t>no</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>SMT_Line_12                   </t>
+  </si>
+  <si>
+    <t>g8_testing_T_L8</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74538F07-B388-4B5D-9587-60CA9861A8F4}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
@@ -516,7 +519,7 @@
   <cols>
     <col min="2" max="2" width="20.796875" customWidth="1"/>
     <col min="3" max="3" width="15.86328125" customWidth="1"/>
-    <col min="4" max="4" width="6.1328125" customWidth="1"/>
+    <col min="4" max="4" width="18.06640625" customWidth="1"/>
     <col min="6" max="6" width="14.53125" customWidth="1"/>
     <col min="7" max="7" width="8.53125" customWidth="1"/>
     <col min="10" max="10" width="36" customWidth="1"/>
@@ -981,6 +984,35 @@
         <v>12</v>
       </c>
     </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16">
+        <v>100</v>
+      </c>
+      <c r="H16" s="1">
+        <v>43822.041666666701</v>
+      </c>
+      <c r="I16" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>